<commit_message>
call it a day
</commit_message>
<xml_diff>
--- a/tables/tables_manual.xlsx
+++ b/tables/tables_manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgw17/Documents/Projects/smdi-manuscript/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D634E68-6613-4B40-B3D7-7409D8C833A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60C95A5-920F-3F4D-A406-B206368A678D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26600" xr2:uid="{32125664-E347-084E-8AA9-096F2A422A2C}"/>
   </bookViews>
@@ -100,9 +100,6 @@
     <t>Comparing the distribution of observed covariates between patients with versus without a value for the partially observed covariate</t>
   </si>
   <si>
-    <t>Assessing the ability to predic missingness based on observed covariates</t>
-  </si>
-  <si>
     <t>Computes the absolute standardized mean differences (ASMD) of patient characteristics between patients with versus without a value for the partially observed covariate(s)</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   <si>
     <t>- ASMD &lt; 0.1: no imbalances in observed patient characteristics; missingness may be likely completely at random or not at random (~MCAR, ~MNAR)
 - ASMD &gt; 0.1: imbalances in observed patient characteristics; missingness may be likely at random (~MAR)</t>
+  </si>
+  <si>
+    <t>Assessing the ability to predict missingness based on observed covariates</t>
   </si>
 </sst>
 </file>
@@ -513,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C8F7A3-13B8-4343-AD3C-75D26A7EA03F}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="204" zoomScaleNormal="204" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="204" zoomScaleNormal="204" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -561,7 +561,7 @@
         <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
@@ -570,7 +570,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -593,7 +593,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -607,7 +607,7 @@
         <v>19</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>15</v>
@@ -616,7 +616,7 @@
         <v>15</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="153" x14ac:dyDescent="0.2">
@@ -627,42 +627,42 @@
         <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added section describing functions
</commit_message>
<xml_diff>
--- a/tables/tables_manual.xlsx
+++ b/tables/tables_manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgw17/Documents/Projects/smdi-manuscript/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60C95A5-920F-3F4D-A406-B206368A678D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBB3435-5BD6-A04D-82FF-3A385ACB03C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26600" xr2:uid="{32125664-E347-084E-8AA9-096F2A422A2C}"/>
   </bookViews>
@@ -82,9 +82,6 @@
     <t>Detailed Hotelling test statistics</t>
   </si>
   <si>
-    <t>Computes Hotelling's multivariate T^2^ t-test for each partially observed covariate, examining patient differences conditional on having an observed covariate value or not.</t>
-  </si>
-  <si>
     <t>Detailed Little's test statistics</t>
   </si>
   <si>
@@ -148,6 +145,9 @@
   </si>
   <si>
     <t>Assessing the ability to predict missingness based on observed covariates</t>
+  </si>
+  <si>
+    <t>Computes Hotelling's multivariate t-test for each partially observed covariate, examining patient differences conditional on having an observed covariate value or not.</t>
   </si>
 </sst>
 </file>
@@ -513,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C8F7A3-13B8-4343-AD3C-75D26A7EA03F}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="204" zoomScaleNormal="204" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="204" zoomScaleNormal="204" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -552,16 +552,16 @@
     </row>
     <row r="2" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>6</v>
@@ -570,21 +570,21 @@
         <v>10</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -593,76 +593,76 @@
         <v>13</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
started with simulation cohort
</commit_message>
<xml_diff>
--- a/tables/tables_manual.xlsx
+++ b/tables/tables_manual.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgw17/Documents/Projects/smdi-manuscript/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBB3435-5BD6-A04D-82FF-3A385ACB03C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A26F339-FFCA-AE40-AD8B-9D05997F748F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="26600" xr2:uid="{32125664-E347-084E-8AA9-096F2A422A2C}"/>
+    <workbookView xWindow="5300" yWindow="500" windowWidth="32640" windowHeight="26600" activeTab="1" xr2:uid="{32125664-E347-084E-8AA9-096F2A422A2C}"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
+    <sheet name="covariates" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="85">
   <si>
     <t>Group</t>
   </si>
@@ -148,19 +149,182 @@
   </si>
   <si>
     <t>Computes Hotelling's multivariate t-test for each partially observed covariate, examining patient differences conditional on having an observed covariate value or not.</t>
+  </si>
+  <si>
+    <t>Associated with exposure/outcome</t>
+  </si>
+  <si>
+    <t>age_num</t>
+  </si>
+  <si>
+    <t>Age at baseline (continuous)</t>
+  </si>
+  <si>
+    <t>Yes/Yes</t>
+  </si>
+  <si>
+    <t>female_cat</t>
+  </si>
+  <si>
+    <t>Female gender (binary)</t>
+  </si>
+  <si>
+    <t>ecog_cat</t>
+  </si>
+  <si>
+    <t>ECOG performance score 0/1 or &gt;1 (binary)</t>
+  </si>
+  <si>
+    <t>MCAR [35%]</t>
+  </si>
+  <si>
+    <t>smoking_cat</t>
+  </si>
+  <si>
+    <t>Smoker vs. non-smoker at baseline (binary)</t>
+  </si>
+  <si>
+    <t>physical_cat</t>
+  </si>
+  <si>
+    <t>Physically active vs not active (binary)</t>
+  </si>
+  <si>
+    <t>egfr_cat</t>
+  </si>
+  <si>
+    <t>EGFR alteration (binary)</t>
+  </si>
+  <si>
+    <t>MAR [40%]</t>
+  </si>
+  <si>
+    <t>alk_cat</t>
+  </si>
+  <si>
+    <t>ALK translocation (binary)</t>
+  </si>
+  <si>
+    <t>No/Yes</t>
+  </si>
+  <si>
+    <t>pdl1_num</t>
+  </si>
+  <si>
+    <t>PD-L1 expression in % (continuous)</t>
+  </si>
+  <si>
+    <t>MNAR(value) [20%]</t>
+  </si>
+  <si>
+    <t>histology_cat</t>
+  </si>
+  <si>
+    <t>Tumor histology squamous vs nonsquamous (binary)</t>
+  </si>
+  <si>
+    <t>ses_cat</t>
+  </si>
+  <si>
+    <t>Socio-economic status (multi-categorical)</t>
+  </si>
+  <si>
+    <t>No/No</t>
+  </si>
+  <si>
+    <t>copd_cat</t>
+  </si>
+  <si>
+    <t>History of COPD (binary)</t>
+  </si>
+  <si>
+    <t>Auxiliary to smoking</t>
+  </si>
+  <si>
+    <t>Variable Name</t>
+  </si>
+  <si>
+    <t>Simulated Missingness [%]</t>
+  </si>
+  <si>
+    <t>Variable Label</t>
+  </si>
+  <si>
+    <t>Age (years)</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>ECOG score</t>
+  </si>
+  <si>
+    <t>Smoking history</t>
+  </si>
+  <si>
+    <t>Physically active</t>
+  </si>
+  <si>
+    <t>EGFR status</t>
+  </si>
+  <si>
+    <t>ALK status</t>
+  </si>
+  <si>
+    <t>PD-L1 expression (%)</t>
+  </si>
+  <si>
+    <t>Tumor histology</t>
+  </si>
+  <si>
+    <t>Socio-economic status</t>
+  </si>
+  <si>
+    <t>History of COPD</t>
+  </si>
+  <si>
+    <t>eventtime</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Deceased</t>
+  </si>
+  <si>
+    <t>Censoring time (years)</t>
+  </si>
+  <si>
+    <t>Indicator if patient experienced outcome</t>
+  </si>
+  <si>
+    <t>Follow-up (years)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF212529"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF212529"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -183,7 +347,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -197,6 +361,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,7 +679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C8F7A3-13B8-4343-AD3C-75D26A7EA03F}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="204" zoomScaleNormal="204" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="204" zoomScaleNormal="204" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -668,4 +834,238 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A17E689-61C8-D24F-9912-7D6392A8FFF8}">
+  <dimension ref="A1:E14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="65.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="6"/>
+    </row>
+    <row r="3" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented SciComms and FDA review feedback, final version for initial submission
</commit_message>
<xml_diff>
--- a/tables/tables_manual.xlsx
+++ b/tables/tables_manual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgw17/Documents/Projects/smdi-manuscript/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A26F339-FFCA-AE40-AD8B-9D05997F748F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0393A540-19CA-BB40-A148-B96C5FBA19FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5300" yWindow="500" windowWidth="32640" windowHeight="26600" activeTab="1" xr2:uid="{32125664-E347-084E-8AA9-096F2A422A2C}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="32640" windowHeight="26600" xr2:uid="{32125664-E347-084E-8AA9-096F2A422A2C}"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
@@ -101,9 +101,6 @@
     <t>Computes the absolute standardized mean differences (ASMD) of patient characteristics between patients with versus without a value for the partially observed covariate(s)</t>
   </si>
   <si>
-    <t>Computes a single global chi-square test statistic across all partially observed covariates with a null hypothesis that the data is missing completely at random.</t>
-  </si>
-  <si>
     <t>Trains and fits a random forest classification model to assess the ability to predict missingness indicator for the partially observed covariate(s).</t>
   </si>
   <si>
@@ -299,6 +296,9 @@
   </si>
   <si>
     <t>Follow-up (years)</t>
+  </si>
+  <si>
+    <t>Computes a single global chi-square test statistic across all partially observed covariates with a null hypothesis that the data are missing completely at random.</t>
   </si>
 </sst>
 </file>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C8F7A3-13B8-4343-AD3C-75D26A7EA03F}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="204" zoomScaleNormal="204" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="204" zoomScaleNormal="204" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -736,7 +736,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -750,7 +750,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -759,7 +759,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="85" x14ac:dyDescent="0.2">
@@ -773,7 +773,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -782,7 +782,7 @@
         <v>14</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="153" x14ac:dyDescent="0.2">
@@ -793,42 +793,42 @@
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -840,7 +840,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A17E689-61C8-D24F-9912-7D6392A8FFF8}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -855,214 +855,214 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>47</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>81</v>
-      </c>
       <c r="C14" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented reviewer # 1 comments
</commit_message>
<xml_diff>
--- a/tables/tables_manual.xlsx
+++ b/tables/tables_manual.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgw17/Documents/Projects/smdi-manuscript/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0393A540-19CA-BB40-A148-B96C5FBA19FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442F27FD-3DA6-5F44-B17D-93544DDB5538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32640" windowHeight="26600" xr2:uid="{32125664-E347-084E-8AA9-096F2A422A2C}"/>
+    <workbookView xWindow="1480" yWindow="500" windowWidth="49720" windowHeight="28300" xr2:uid="{32125664-E347-084E-8AA9-096F2A422A2C}"/>
   </bookViews>
   <sheets>
     <sheet name="table1" sheetId="1" r:id="rId1"/>
     <sheet name="covariates" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -679,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05C8F7A3-13B8-4343-AD3C-75D26A7EA03F}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="204" zoomScaleNormal="204" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -739,7 +739,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -762,7 +762,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -785,7 +785,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -808,7 +808,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
changed 'logistic' to glm after the update of the function
</commit_message>
<xml_diff>
--- a/tables/tables_manual.xlsx
+++ b/tables/tables_manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgw17/Documents/Projects/smdi-manuscript/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442F27FD-3DA6-5F44-B17D-93544DDB5538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79ECCF30-F055-9141-88E5-27B922E2EA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="500" windowWidth="49720" windowHeight="28300" xr2:uid="{32125664-E347-084E-8AA9-096F2A422A2C}"/>
   </bookViews>
@@ -127,9 +127,6 @@
     <t>Evaluates whether missingness of a covariate is associated with the outcome</t>
   </si>
   <si>
-    <t>Fits outcome model (linear, logistic or proportional hazards depending on the outcome under study) with the missingness indicator of the partially observed covariate(s). The estimates are computed both as a univariate model (just considering the missingness indicator) and an adjusted model with all covariates in the dataset.</t>
-  </si>
-  <si>
     <t xml:space="preserve">- No association in either univariate or adjusted model and no meaningful difference in the log HR after full adjustment (~MCAR). 
 - Association in univariate but not fully adjusted model (~MAR). 
 - Meaningful difference in the log HR also after full adjustment (~MNAR). </t>
@@ -299,6 +296,9 @@
   </si>
   <si>
     <t>Computes a single global chi-square test statistic across all partially observed covariates with a null hypothesis that the data are missing completely at random.</t>
+  </si>
+  <si>
+    <t>Fits outcome model (linear, glm or proportional hazards depending on the outcome under study) with the missingness indicator of the partially observed covariate(s). The estimates are computed both as a univariate model (just considering the missingness indicator) and an adjusted model with all covariates in the dataset.</t>
   </si>
 </sst>
 </file>
@@ -680,7 +680,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -736,7 +736,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -750,7 +750,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -773,7 +773,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -785,7 +785,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="102" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -793,7 +793,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>20</v>
@@ -808,7 +808,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="153" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -819,16 +819,16 @@
         <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -855,214 +855,214 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>39</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>52</v>
       </c>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>57</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>80</v>
-      </c>
       <c r="C14" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished reviewer #2 review and finalized all responses, supplement and manuscript updates.Sending revised version now to  co-author review.
</commit_message>
<xml_diff>
--- a/tables/tables_manual.xlsx
+++ b/tables/tables_manual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgw17/Documents/Projects/smdi-manuscript/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79ECCF30-F055-9141-88E5-27B922E2EA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A441B7-3AE2-1F4C-903C-CCB33455C7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="500" windowWidth="49720" windowHeight="28300" xr2:uid="{32125664-E347-084E-8AA9-096F2A422A2C}"/>
   </bookViews>
@@ -107,10 +107,6 @@
     <t>Aggregated summary table with the area under the receiver operating characteristic curve (AUC) value for each partially observed covariate</t>
   </si>
   <si>
-    <t>- Individual AUC value
-- ggplot2 figure illustrating the variable importance for the prediction made expressed by the mean decrease in accuracy per predictor</t>
-  </si>
-  <si>
     <t>- AUC values ~ 0.5 indicate completely random or not at random prediction (~MCAR, ~MNAR)
 - Values meaningfully above 0.5 indicate stronger relationships between covariates and missingness (~MAR)</t>
   </si>
@@ -299,6 +295,11 @@
   </si>
   <si>
     <t>Fits outcome model (linear, glm or proportional hazards depending on the outcome under study) with the missingness indicator of the partially observed covariate(s). The estimates are computed both as a univariate model (just considering the missingness indicator) and an adjusted model with all covariates in the dataset.</t>
+  </si>
+  <si>
+    <t>- Individual AUC value
+- ggplot2 figure illustrating the variable importance for the prediction made expressed by the mean decrease in accuracy per predictor
+- Estimated out-of-bag (OOB) error</t>
   </si>
 </sst>
 </file>
@@ -680,7 +681,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -736,7 +737,7 @@
         <v>10</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -750,7 +751,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -759,7 +760,7 @@
         <v>13</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -773,7 +774,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>14</v>
@@ -782,7 +783,7 @@
         <v>14</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="153" x14ac:dyDescent="0.2">
@@ -793,7 +794,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>20</v>
@@ -802,33 +803,33 @@
         <v>21</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -855,214 +856,214 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>36</v>
       </c>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>38</v>
-      </c>
       <c r="D3" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>45</v>
-      </c>
       <c r="D6" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E6" s="6"/>
     </row>
     <row r="7" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>50</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>51</v>
       </c>
       <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>53</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="C14" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>